<commit_message>
UPD FOLDER TOYOTA Entrega Miry
</commit_message>
<xml_diff>
--- a/TOYOTA-Celaya/Fuentes - Toyota/Distribuidor/Admon/Atn Clientes/Toyota - CEL - Analisis - Atencion a Clientes.xlsx
+++ b/TOYOTA-Celaya/Fuentes - Toyota/Distribuidor/Admon/Atn Clientes/Toyota - CEL - Analisis - Atencion a Clientes.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KE\JMM\PROCESSES MAPPING\toyota_proceso\TOYOTA-Celaya\Fuentes - Toyota\Distribuidor\Admon\Atn Clientes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFFEA979-EA16-48B7-845E-A214F0F42A83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F62F837-32A0-4350-840B-CF47312AC5D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="330" yWindow="30" windowWidth="19950" windowHeight="10800" xr2:uid="{7E74557B-02A4-44EF-8F45-FC026D5565D6}"/>
+    <workbookView xWindow="360" yWindow="165" windowWidth="19950" windowHeight="10590" activeTab="1" xr2:uid="{7E74557B-02A4-44EF-8F45-FC026D5565D6}"/>
   </bookViews>
   <sheets>
     <sheet name="FTO Task List" sheetId="4" r:id="rId1"/>
+    <sheet name="FTO Data List" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="119">
   <si>
     <t>Tipo</t>
   </si>
@@ -277,9 +278,15 @@
     <t>Se revisa el Kepler orden por orden y se pasa  manualmente a un archivo de excel para gestion  del PSFU.</t>
   </si>
   <si>
+    <t>- BD Formato Seguimiento PSFU {YYYY}.xlsx 
+Ver preliminarmente ( porque 2023 no esta completado, se estan agragando controles de los nuevos programas Toyota ) : 
+BD Formato Seguimiento PSFU 2022.xlsx 
+Hojas mes Diciembre : Hoja Graficos  señalizada por colores en Hoja BD, para determinar los Conteos.</t>
+  </si>
+  <si>
     <t>- K75 maneja 5 preguntas y Toyota maneja 3, ya esta especificadas.
 - Agregar Campos ( x Orden ) : 
-+ Estatus de Satisfaccion (3 valores Hoja BD - M) 
++ Estatus de Satisfaccion (3 valores Hoja BD - K) 
 + Semana (AUTO en base a Fecha Cierre Orden , Hoja BD - B)
 + Agregar 3 Fechas de Contacto ( Intentos ) 
 + Puntuacion Medallia 
@@ -289,20 +296,216 @@
 + Responable Nota ( CAT Contactos / Empleados )
 + Comentarios CLIENTE
 + Comentarios ATN CLIE 
-+ Estatus Nota ( ATN CLIE ; Hoja BD - V )</t>
-  </si>
-  <si>
-    <t>- BD Formato Seguimiento PSFU {YYYY}.xlsx 
-Ver preliminarmente ( porque 2023 no esta completado, se estan agragando controles de los nuevos programas Toyota ) : 
-BD Formato Seguimiento PSFU 2022.xlsx 
-Hojas mes Diciembre : Hoja Graficos  señalizada por colores en Hoja BD, para determinar los Conteos.</t>
++ Estatus Nota ( ATN CLIE ; CAT Hoja BD Noviembre - V )</t>
+  </si>
+  <si>
+    <t>T - Texto
+N - Entero
+D - Decimal
+F - Fecha
+H - Hora
+FH - F &amp; H
+S - Flag / ST
+C - Catalogo
+R - Control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V - Ventas
+S - Servicio
+</t>
+  </si>
+  <si>
+    <t>A - A,B,C
+V - View</t>
+  </si>
+  <si>
+    <t>K - K75
+T - Toyota
+D - DISTR</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Type Aux</t>
+  </si>
+  <si>
+    <t>TBL - Entity</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Usage</t>
+  </si>
+  <si>
+    <t>Mandatory</t>
+  </si>
+  <si>
+    <t>ID Task</t>
+  </si>
+  <si>
+    <t>K75</t>
+  </si>
+  <si>
+    <t>K75 - Ref</t>
+  </si>
+  <si>
+    <t>APP</t>
+  </si>
+  <si>
+    <t>APP - Ref</t>
+  </si>
+  <si>
+    <t>TOY</t>
+  </si>
+  <si>
+    <t>TOY Ref</t>
+  </si>
+  <si>
+    <t>DISTR</t>
+  </si>
+  <si>
+    <t>DISTR - Ref</t>
+  </si>
+  <si>
+    <t>DMS</t>
+  </si>
+  <si>
+    <t>Cobertura</t>
+  </si>
+  <si>
+    <t>DMS - Ref</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Pregunta 1 FIRM</t>
+  </si>
+  <si>
+    <t>Pregunta 2 FIRM</t>
+  </si>
+  <si>
+    <t>Pregunta 3 FIRM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿Su vehículo fue reparado correctamente desde la primera vez? </t>
+  </si>
+  <si>
+    <t>¿Fue completada la reparación en el tiempo estimado?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿La reparacion se hizo en un tiempo razonable? </t>
+  </si>
+  <si>
+    <t>S - AC - 001</t>
+  </si>
+  <si>
+    <t>OLUS</t>
+  </si>
+  <si>
+    <t>Estatus Satisfaccion</t>
+  </si>
+  <si>
+    <t>Orden</t>
+  </si>
+  <si>
+    <t>Atn Clientes</t>
+  </si>
+  <si>
+    <t>Semana Reporte</t>
+  </si>
+  <si>
+    <t>Calculo - Semana</t>
+  </si>
+  <si>
+    <t>Semana Determinada de la Fecha de Cierre de la Orden</t>
+  </si>
+  <si>
+    <t>Contacto 1</t>
+  </si>
+  <si>
+    <t>FH</t>
+  </si>
+  <si>
+    <t>Contacto 2</t>
+  </si>
+  <si>
+    <t>Contacto 3</t>
+  </si>
+  <si>
+    <t>Intentos de Contacto al Cliente</t>
+  </si>
+  <si>
+    <t>Excel</t>
+  </si>
+  <si>
+    <t>Puntuacion Medallia</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>1 .. 5</t>
+  </si>
+  <si>
+    <t>Rango de Calificacion de la Encuesta de Satisfaccion que se hace via WEB</t>
+  </si>
+  <si>
+    <t>Tipo Nota</t>
+  </si>
+  <si>
+    <t>Motivo Nota</t>
+  </si>
+  <si>
+    <t>Departamento Nota</t>
+  </si>
+  <si>
+    <t>Responsible Nota</t>
+  </si>
+  <si>
+    <t>Estatus Nota</t>
+  </si>
+  <si>
+    <t>Comentarios Cliente</t>
+  </si>
+  <si>
+    <t>Comentarios ATN Clientes</t>
+  </si>
+  <si>
+    <t>Notas de la Llamada (por lo regular quejas)</t>
+  </si>
+  <si>
+    <t>Comentarios que hace el Cliente</t>
+  </si>
+  <si>
+    <t>Comentarios que hace el area de atencion a clientes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -363,8 +566,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -461,6 +670,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -474,7 +701,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -536,6 +763,55 @@
     <xf numFmtId="49" fontId="2" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -852,8 +1128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D038D82-D5B0-455D-8135-9E8D2F22CF22}">
   <dimension ref="B2:AB11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AA5" sqref="AA5"/>
+    <sheetView topLeftCell="V4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Z5" sqref="Z5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,7 +1158,7 @@
     <col min="22" max="22" width="15.5703125" style="3" customWidth="1"/>
     <col min="23" max="23" width="18.5703125" style="3" customWidth="1"/>
     <col min="24" max="25" width="24.42578125" style="3" customWidth="1"/>
-    <col min="26" max="26" width="47.85546875" style="3" customWidth="1"/>
+    <col min="26" max="26" width="48.42578125" style="3" customWidth="1"/>
     <col min="27" max="27" width="41.85546875" style="3" customWidth="1"/>
     <col min="28" max="28" width="16.5703125" style="3" customWidth="1"/>
     <col min="29" max="16384" width="9.140625" style="3"/>
@@ -1121,12 +1397,14 @@
         <v>49</v>
       </c>
       <c r="Z5" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA5" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="AA5" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB5" s="15"/>
+      <c r="AB5" s="15" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="6" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B6" s="11"/>
@@ -1317,4 +1595,888 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B1508E8-2F4F-40ED-86F2-121428015636}">
+  <dimension ref="B2:X21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="21" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="21" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="21" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="21" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="21" customWidth="1"/>
+    <col min="8" max="8" width="53" style="21" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="21" customWidth="1"/>
+    <col min="10" max="11" width="13.140625" style="21" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" style="21" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" style="21" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" style="21" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" style="21" customWidth="1"/>
+    <col min="16" max="16" width="6.7109375" style="21" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" style="21" customWidth="1"/>
+    <col min="18" max="18" width="8" style="21" customWidth="1"/>
+    <col min="19" max="19" width="14.42578125" style="21" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" style="23"/>
+    <col min="21" max="21" width="11.7109375" style="23" customWidth="1"/>
+    <col min="22" max="22" width="10.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="9.140625" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:24" ht="135" x14ac:dyDescent="0.25">
+      <c r="C2" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="K2" s="22"/>
+      <c r="U2" s="22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B3" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="J3" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="K3" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="L3" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="M3" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="N3" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="O3" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="P3" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q3" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="R3" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="S3" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="T3" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="U3" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="V3" s="33" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="2:24" s="37" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="K4" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
+      <c r="P4" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q4" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="R4" s="34"/>
+      <c r="S4" s="34"/>
+      <c r="T4" s="36"/>
+      <c r="U4" s="36"/>
+      <c r="V4" s="36"/>
+      <c r="W4" s="36"/>
+      <c r="X4" s="36"/>
+    </row>
+    <row r="5" spans="2:24" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="K5" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q5" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="R5" s="34"/>
+      <c r="S5" s="34"/>
+      <c r="T5" s="36"/>
+      <c r="U5" s="36"/>
+      <c r="V5" s="36"/>
+      <c r="W5" s="36"/>
+      <c r="X5" s="36"/>
+    </row>
+    <row r="6" spans="2:24" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="K6" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="N6" s="34"/>
+      <c r="O6" s="34"/>
+      <c r="P6" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q6" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="R6" s="34"/>
+      <c r="S6" s="34"/>
+      <c r="T6" s="36"/>
+      <c r="U6" s="36"/>
+      <c r="V6" s="36"/>
+      <c r="W6" s="36"/>
+      <c r="X6" s="36"/>
+    </row>
+    <row r="7" spans="2:24" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F7" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="N7" s="34"/>
+      <c r="O7" s="34"/>
+      <c r="P7" s="34"/>
+      <c r="Q7" s="34"/>
+      <c r="R7" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="S7" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="T7" s="36"/>
+      <c r="U7" s="36"/>
+      <c r="V7" s="36"/>
+      <c r="W7" s="36"/>
+      <c r="X7" s="36"/>
+    </row>
+    <row r="8" spans="2:24" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F8" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="H8" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="L8" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="M8" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="N8" s="34"/>
+      <c r="O8" s="34"/>
+      <c r="P8" s="34"/>
+      <c r="Q8" s="34"/>
+      <c r="R8" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="S8" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="T8" s="36"/>
+      <c r="U8" s="36"/>
+      <c r="V8" s="36"/>
+      <c r="W8" s="36"/>
+      <c r="X8" s="36"/>
+    </row>
+    <row r="9" spans="2:24" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F9" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="H9" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
+      <c r="P9" s="34"/>
+      <c r="Q9" s="34"/>
+      <c r="R9" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="S9" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="T9" s="36"/>
+      <c r="U9" s="36"/>
+      <c r="V9" s="36"/>
+      <c r="W9" s="36"/>
+      <c r="X9" s="36"/>
+    </row>
+    <row r="10" spans="2:24" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F10" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="H10" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="N10" s="34"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="34"/>
+      <c r="Q10" s="34"/>
+      <c r="R10" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="S10" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="T10" s="36"/>
+      <c r="U10" s="36"/>
+      <c r="V10" s="36"/>
+      <c r="W10" s="36"/>
+      <c r="X10" s="36"/>
+    </row>
+    <row r="11" spans="2:24" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F11" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="H11" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="N11" s="34"/>
+      <c r="O11" s="34"/>
+      <c r="P11" s="34"/>
+      <c r="Q11" s="34"/>
+      <c r="R11" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="S11" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="T11" s="36"/>
+      <c r="U11" s="36"/>
+      <c r="V11" s="36"/>
+      <c r="W11" s="36"/>
+      <c r="X11" s="36"/>
+    </row>
+    <row r="12" spans="2:24" s="37" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F12" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="H12" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="N12" s="34"/>
+      <c r="O12" s="34"/>
+      <c r="P12" s="34"/>
+      <c r="Q12" s="34"/>
+      <c r="R12" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="S12" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="T12" s="36"/>
+      <c r="U12" s="36"/>
+      <c r="V12" s="36"/>
+      <c r="W12" s="36"/>
+      <c r="X12" s="36"/>
+    </row>
+    <row r="13" spans="2:24" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F13" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="H13" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="N13" s="34"/>
+      <c r="O13" s="34"/>
+      <c r="P13" s="34"/>
+      <c r="Q13" s="34"/>
+      <c r="R13" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="S13" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="T13" s="36"/>
+      <c r="U13" s="36"/>
+      <c r="V13" s="36"/>
+      <c r="W13" s="36"/>
+      <c r="X13" s="36"/>
+    </row>
+    <row r="14" spans="2:24" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F14" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="H14" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="N14" s="34"/>
+      <c r="O14" s="34"/>
+      <c r="P14" s="34"/>
+      <c r="Q14" s="34"/>
+      <c r="R14" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="S14" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="T14" s="36"/>
+      <c r="U14" s="36"/>
+      <c r="V14" s="36"/>
+      <c r="W14" s="36"/>
+      <c r="X14" s="36"/>
+    </row>
+    <row r="15" spans="2:24" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F15" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="H15" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="L15" s="34"/>
+      <c r="M15" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="N15" s="34"/>
+      <c r="O15" s="34"/>
+      <c r="P15" s="34"/>
+      <c r="Q15" s="34"/>
+      <c r="R15" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="S15" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="T15" s="36"/>
+      <c r="U15" s="36"/>
+      <c r="V15" s="36"/>
+      <c r="W15" s="36"/>
+      <c r="X15" s="36"/>
+    </row>
+    <row r="16" spans="2:24" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="H16" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="N16" s="34"/>
+      <c r="O16" s="34"/>
+      <c r="P16" s="34"/>
+      <c r="Q16" s="34"/>
+      <c r="R16" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="S16" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="T16" s="36"/>
+      <c r="U16" s="36"/>
+      <c r="V16" s="36"/>
+      <c r="W16" s="36"/>
+      <c r="X16" s="36"/>
+    </row>
+    <row r="17" spans="2:24" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F17" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="H17" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="L17" s="34"/>
+      <c r="M17" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="N17" s="34"/>
+      <c r="O17" s="34"/>
+      <c r="P17" s="34"/>
+      <c r="Q17" s="34"/>
+      <c r="R17" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="S17" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="T17" s="36"/>
+      <c r="U17" s="36"/>
+      <c r="V17" s="36"/>
+      <c r="W17" s="36"/>
+      <c r="X17" s="36"/>
+    </row>
+    <row r="18" spans="2:24" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F18" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="H18" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="L18" s="34"/>
+      <c r="M18" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="N18" s="34"/>
+      <c r="O18" s="34"/>
+      <c r="P18" s="34"/>
+      <c r="Q18" s="34"/>
+      <c r="R18" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="S18" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="T18" s="36"/>
+      <c r="U18" s="36"/>
+      <c r="V18" s="36"/>
+      <c r="W18" s="36"/>
+      <c r="X18" s="36"/>
+    </row>
+    <row r="19" spans="2:24" s="37" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F19" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="H19" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="L19" s="34"/>
+      <c r="M19" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="N19" s="34"/>
+      <c r="O19" s="34"/>
+      <c r="P19" s="34"/>
+      <c r="Q19" s="34"/>
+      <c r="R19" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="S19" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="T19" s="36"/>
+      <c r="U19" s="36"/>
+      <c r="V19" s="36"/>
+      <c r="W19" s="36"/>
+      <c r="X19" s="36"/>
+    </row>
+    <row r="20" spans="2:24" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="34"/>
+      <c r="N20" s="34"/>
+      <c r="O20" s="34"/>
+      <c r="P20" s="34"/>
+      <c r="Q20" s="34"/>
+      <c r="R20" s="34"/>
+      <c r="S20" s="34"/>
+      <c r="T20" s="36"/>
+      <c r="U20" s="36"/>
+      <c r="V20" s="36"/>
+      <c r="W20" s="36"/>
+      <c r="X20" s="36"/>
+    </row>
+    <row r="21" spans="2:24" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="34"/>
+      <c r="N21" s="34"/>
+      <c r="O21" s="34"/>
+      <c r="P21" s="34"/>
+      <c r="Q21" s="34"/>
+      <c r="R21" s="34"/>
+      <c r="S21" s="34"/>
+      <c r="T21" s="36"/>
+      <c r="U21" s="36"/>
+      <c r="V21" s="36"/>
+      <c r="W21" s="36"/>
+      <c r="X21" s="36"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Carpeta de Trabajo - CELAYA - 20030427 1840 - ENTREGA MIRY
</commit_message>
<xml_diff>
--- a/TOYOTA-Celaya/Fuentes - Toyota/Distribuidor/Admon/Atn Clientes/Toyota - CEL - Analisis - Atencion a Clientes.xlsx
+++ b/TOYOTA-Celaya/Fuentes - Toyota/Distribuidor/Admon/Atn Clientes/Toyota - CEL - Analisis - Atencion a Clientes.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KE\JMM\PROCESSES MAPPING\toyota_proceso\TOYOTA-Celaya\Fuentes - Toyota\Distribuidor\Admon\Atn Clientes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFFEA979-EA16-48B7-845E-A214F0F42A83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F62F837-32A0-4350-840B-CF47312AC5D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="330" yWindow="30" windowWidth="19950" windowHeight="10800" xr2:uid="{7E74557B-02A4-44EF-8F45-FC026D5565D6}"/>
+    <workbookView xWindow="360" yWindow="165" windowWidth="19950" windowHeight="10590" activeTab="1" xr2:uid="{7E74557B-02A4-44EF-8F45-FC026D5565D6}"/>
   </bookViews>
   <sheets>
     <sheet name="FTO Task List" sheetId="4" r:id="rId1"/>
+    <sheet name="FTO Data List" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="119">
   <si>
     <t>Tipo</t>
   </si>
@@ -277,9 +278,15 @@
     <t>Se revisa el Kepler orden por orden y se pasa  manualmente a un archivo de excel para gestion  del PSFU.</t>
   </si>
   <si>
+    <t>- BD Formato Seguimiento PSFU {YYYY}.xlsx 
+Ver preliminarmente ( porque 2023 no esta completado, se estan agragando controles de los nuevos programas Toyota ) : 
+BD Formato Seguimiento PSFU 2022.xlsx 
+Hojas mes Diciembre : Hoja Graficos  señalizada por colores en Hoja BD, para determinar los Conteos.</t>
+  </si>
+  <si>
     <t>- K75 maneja 5 preguntas y Toyota maneja 3, ya esta especificadas.
 - Agregar Campos ( x Orden ) : 
-+ Estatus de Satisfaccion (3 valores Hoja BD - M) 
++ Estatus de Satisfaccion (3 valores Hoja BD - K) 
 + Semana (AUTO en base a Fecha Cierre Orden , Hoja BD - B)
 + Agregar 3 Fechas de Contacto ( Intentos ) 
 + Puntuacion Medallia 
@@ -289,20 +296,216 @@
 + Responable Nota ( CAT Contactos / Empleados )
 + Comentarios CLIENTE
 + Comentarios ATN CLIE 
-+ Estatus Nota ( ATN CLIE ; Hoja BD - V )</t>
-  </si>
-  <si>
-    <t>- BD Formato Seguimiento PSFU {YYYY}.xlsx 
-Ver preliminarmente ( porque 2023 no esta completado, se estan agragando controles de los nuevos programas Toyota ) : 
-BD Formato Seguimiento PSFU 2022.xlsx 
-Hojas mes Diciembre : Hoja Graficos  señalizada por colores en Hoja BD, para determinar los Conteos.</t>
++ Estatus Nota ( ATN CLIE ; CAT Hoja BD Noviembre - V )</t>
+  </si>
+  <si>
+    <t>T - Texto
+N - Entero
+D - Decimal
+F - Fecha
+H - Hora
+FH - F &amp; H
+S - Flag / ST
+C - Catalogo
+R - Control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V - Ventas
+S - Servicio
+</t>
+  </si>
+  <si>
+    <t>A - A,B,C
+V - View</t>
+  </si>
+  <si>
+    <t>K - K75
+T - Toyota
+D - DISTR</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Type Aux</t>
+  </si>
+  <si>
+    <t>TBL - Entity</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Usage</t>
+  </si>
+  <si>
+    <t>Mandatory</t>
+  </si>
+  <si>
+    <t>ID Task</t>
+  </si>
+  <si>
+    <t>K75</t>
+  </si>
+  <si>
+    <t>K75 - Ref</t>
+  </si>
+  <si>
+    <t>APP</t>
+  </si>
+  <si>
+    <t>APP - Ref</t>
+  </si>
+  <si>
+    <t>TOY</t>
+  </si>
+  <si>
+    <t>TOY Ref</t>
+  </si>
+  <si>
+    <t>DISTR</t>
+  </si>
+  <si>
+    <t>DISTR - Ref</t>
+  </si>
+  <si>
+    <t>DMS</t>
+  </si>
+  <si>
+    <t>Cobertura</t>
+  </si>
+  <si>
+    <t>DMS - Ref</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Pregunta 1 FIRM</t>
+  </si>
+  <si>
+    <t>Pregunta 2 FIRM</t>
+  </si>
+  <si>
+    <t>Pregunta 3 FIRM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿Su vehículo fue reparado correctamente desde la primera vez? </t>
+  </si>
+  <si>
+    <t>¿Fue completada la reparación en el tiempo estimado?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿La reparacion se hizo en un tiempo razonable? </t>
+  </si>
+  <si>
+    <t>S - AC - 001</t>
+  </si>
+  <si>
+    <t>OLUS</t>
+  </si>
+  <si>
+    <t>Estatus Satisfaccion</t>
+  </si>
+  <si>
+    <t>Orden</t>
+  </si>
+  <si>
+    <t>Atn Clientes</t>
+  </si>
+  <si>
+    <t>Semana Reporte</t>
+  </si>
+  <si>
+    <t>Calculo - Semana</t>
+  </si>
+  <si>
+    <t>Semana Determinada de la Fecha de Cierre de la Orden</t>
+  </si>
+  <si>
+    <t>Contacto 1</t>
+  </si>
+  <si>
+    <t>FH</t>
+  </si>
+  <si>
+    <t>Contacto 2</t>
+  </si>
+  <si>
+    <t>Contacto 3</t>
+  </si>
+  <si>
+    <t>Intentos de Contacto al Cliente</t>
+  </si>
+  <si>
+    <t>Excel</t>
+  </si>
+  <si>
+    <t>Puntuacion Medallia</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>1 .. 5</t>
+  </si>
+  <si>
+    <t>Rango de Calificacion de la Encuesta de Satisfaccion que se hace via WEB</t>
+  </si>
+  <si>
+    <t>Tipo Nota</t>
+  </si>
+  <si>
+    <t>Motivo Nota</t>
+  </si>
+  <si>
+    <t>Departamento Nota</t>
+  </si>
+  <si>
+    <t>Responsible Nota</t>
+  </si>
+  <si>
+    <t>Estatus Nota</t>
+  </si>
+  <si>
+    <t>Comentarios Cliente</t>
+  </si>
+  <si>
+    <t>Comentarios ATN Clientes</t>
+  </si>
+  <si>
+    <t>Notas de la Llamada (por lo regular quejas)</t>
+  </si>
+  <si>
+    <t>Comentarios que hace el Cliente</t>
+  </si>
+  <si>
+    <t>Comentarios que hace el area de atencion a clientes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -363,8 +566,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -461,6 +670,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -474,7 +701,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -536,6 +763,55 @@
     <xf numFmtId="49" fontId="2" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -852,8 +1128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D038D82-D5B0-455D-8135-9E8D2F22CF22}">
   <dimension ref="B2:AB11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AA5" sqref="AA5"/>
+    <sheetView topLeftCell="V4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Z5" sqref="Z5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,7 +1158,7 @@
     <col min="22" max="22" width="15.5703125" style="3" customWidth="1"/>
     <col min="23" max="23" width="18.5703125" style="3" customWidth="1"/>
     <col min="24" max="25" width="24.42578125" style="3" customWidth="1"/>
-    <col min="26" max="26" width="47.85546875" style="3" customWidth="1"/>
+    <col min="26" max="26" width="48.42578125" style="3" customWidth="1"/>
     <col min="27" max="27" width="41.85546875" style="3" customWidth="1"/>
     <col min="28" max="28" width="16.5703125" style="3" customWidth="1"/>
     <col min="29" max="16384" width="9.140625" style="3"/>
@@ -1121,12 +1397,14 @@
         <v>49</v>
       </c>
       <c r="Z5" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA5" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="AA5" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB5" s="15"/>
+      <c r="AB5" s="15" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="6" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B6" s="11"/>
@@ -1317,4 +1595,888 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B1508E8-2F4F-40ED-86F2-121428015636}">
+  <dimension ref="B2:X21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="21" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="21" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="21" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="21" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="21" customWidth="1"/>
+    <col min="8" max="8" width="53" style="21" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="21" customWidth="1"/>
+    <col min="10" max="11" width="13.140625" style="21" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" style="21" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" style="21" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" style="21" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" style="21" customWidth="1"/>
+    <col min="16" max="16" width="6.7109375" style="21" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" style="21" customWidth="1"/>
+    <col min="18" max="18" width="8" style="21" customWidth="1"/>
+    <col min="19" max="19" width="14.42578125" style="21" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" style="23"/>
+    <col min="21" max="21" width="11.7109375" style="23" customWidth="1"/>
+    <col min="22" max="22" width="10.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="9.140625" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:24" ht="135" x14ac:dyDescent="0.25">
+      <c r="C2" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="K2" s="22"/>
+      <c r="U2" s="22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B3" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="J3" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="K3" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="L3" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="M3" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="N3" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="O3" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="P3" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q3" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="R3" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="S3" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="T3" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="U3" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="V3" s="33" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="2:24" s="37" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="K4" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
+      <c r="P4" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q4" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="R4" s="34"/>
+      <c r="S4" s="34"/>
+      <c r="T4" s="36"/>
+      <c r="U4" s="36"/>
+      <c r="V4" s="36"/>
+      <c r="W4" s="36"/>
+      <c r="X4" s="36"/>
+    </row>
+    <row r="5" spans="2:24" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="K5" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q5" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="R5" s="34"/>
+      <c r="S5" s="34"/>
+      <c r="T5" s="36"/>
+      <c r="U5" s="36"/>
+      <c r="V5" s="36"/>
+      <c r="W5" s="36"/>
+      <c r="X5" s="36"/>
+    </row>
+    <row r="6" spans="2:24" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="K6" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="N6" s="34"/>
+      <c r="O6" s="34"/>
+      <c r="P6" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q6" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="R6" s="34"/>
+      <c r="S6" s="34"/>
+      <c r="T6" s="36"/>
+      <c r="U6" s="36"/>
+      <c r="V6" s="36"/>
+      <c r="W6" s="36"/>
+      <c r="X6" s="36"/>
+    </row>
+    <row r="7" spans="2:24" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F7" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="N7" s="34"/>
+      <c r="O7" s="34"/>
+      <c r="P7" s="34"/>
+      <c r="Q7" s="34"/>
+      <c r="R7" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="S7" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="T7" s="36"/>
+      <c r="U7" s="36"/>
+      <c r="V7" s="36"/>
+      <c r="W7" s="36"/>
+      <c r="X7" s="36"/>
+    </row>
+    <row r="8" spans="2:24" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F8" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="H8" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="L8" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="M8" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="N8" s="34"/>
+      <c r="O8" s="34"/>
+      <c r="P8" s="34"/>
+      <c r="Q8" s="34"/>
+      <c r="R8" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="S8" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="T8" s="36"/>
+      <c r="U8" s="36"/>
+      <c r="V8" s="36"/>
+      <c r="W8" s="36"/>
+      <c r="X8" s="36"/>
+    </row>
+    <row r="9" spans="2:24" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F9" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="H9" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
+      <c r="P9" s="34"/>
+      <c r="Q9" s="34"/>
+      <c r="R9" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="S9" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="T9" s="36"/>
+      <c r="U9" s="36"/>
+      <c r="V9" s="36"/>
+      <c r="W9" s="36"/>
+      <c r="X9" s="36"/>
+    </row>
+    <row r="10" spans="2:24" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F10" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="H10" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="N10" s="34"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="34"/>
+      <c r="Q10" s="34"/>
+      <c r="R10" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="S10" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="T10" s="36"/>
+      <c r="U10" s="36"/>
+      <c r="V10" s="36"/>
+      <c r="W10" s="36"/>
+      <c r="X10" s="36"/>
+    </row>
+    <row r="11" spans="2:24" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F11" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="H11" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="N11" s="34"/>
+      <c r="O11" s="34"/>
+      <c r="P11" s="34"/>
+      <c r="Q11" s="34"/>
+      <c r="R11" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="S11" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="T11" s="36"/>
+      <c r="U11" s="36"/>
+      <c r="V11" s="36"/>
+      <c r="W11" s="36"/>
+      <c r="X11" s="36"/>
+    </row>
+    <row r="12" spans="2:24" s="37" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F12" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="H12" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="N12" s="34"/>
+      <c r="O12" s="34"/>
+      <c r="P12" s="34"/>
+      <c r="Q12" s="34"/>
+      <c r="R12" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="S12" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="T12" s="36"/>
+      <c r="U12" s="36"/>
+      <c r="V12" s="36"/>
+      <c r="W12" s="36"/>
+      <c r="X12" s="36"/>
+    </row>
+    <row r="13" spans="2:24" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F13" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="H13" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="N13" s="34"/>
+      <c r="O13" s="34"/>
+      <c r="P13" s="34"/>
+      <c r="Q13" s="34"/>
+      <c r="R13" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="S13" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="T13" s="36"/>
+      <c r="U13" s="36"/>
+      <c r="V13" s="36"/>
+      <c r="W13" s="36"/>
+      <c r="X13" s="36"/>
+    </row>
+    <row r="14" spans="2:24" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F14" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="H14" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="N14" s="34"/>
+      <c r="O14" s="34"/>
+      <c r="P14" s="34"/>
+      <c r="Q14" s="34"/>
+      <c r="R14" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="S14" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="T14" s="36"/>
+      <c r="U14" s="36"/>
+      <c r="V14" s="36"/>
+      <c r="W14" s="36"/>
+      <c r="X14" s="36"/>
+    </row>
+    <row r="15" spans="2:24" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F15" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="H15" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="L15" s="34"/>
+      <c r="M15" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="N15" s="34"/>
+      <c r="O15" s="34"/>
+      <c r="P15" s="34"/>
+      <c r="Q15" s="34"/>
+      <c r="R15" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="S15" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="T15" s="36"/>
+      <c r="U15" s="36"/>
+      <c r="V15" s="36"/>
+      <c r="W15" s="36"/>
+      <c r="X15" s="36"/>
+    </row>
+    <row r="16" spans="2:24" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="H16" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="N16" s="34"/>
+      <c r="O16" s="34"/>
+      <c r="P16" s="34"/>
+      <c r="Q16" s="34"/>
+      <c r="R16" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="S16" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="T16" s="36"/>
+      <c r="U16" s="36"/>
+      <c r="V16" s="36"/>
+      <c r="W16" s="36"/>
+      <c r="X16" s="36"/>
+    </row>
+    <row r="17" spans="2:24" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F17" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="H17" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="L17" s="34"/>
+      <c r="M17" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="N17" s="34"/>
+      <c r="O17" s="34"/>
+      <c r="P17" s="34"/>
+      <c r="Q17" s="34"/>
+      <c r="R17" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="S17" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="T17" s="36"/>
+      <c r="U17" s="36"/>
+      <c r="V17" s="36"/>
+      <c r="W17" s="36"/>
+      <c r="X17" s="36"/>
+    </row>
+    <row r="18" spans="2:24" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F18" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="H18" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="L18" s="34"/>
+      <c r="M18" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="N18" s="34"/>
+      <c r="O18" s="34"/>
+      <c r="P18" s="34"/>
+      <c r="Q18" s="34"/>
+      <c r="R18" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="S18" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="T18" s="36"/>
+      <c r="U18" s="36"/>
+      <c r="V18" s="36"/>
+      <c r="W18" s="36"/>
+      <c r="X18" s="36"/>
+    </row>
+    <row r="19" spans="2:24" s="37" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F19" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="H19" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="L19" s="34"/>
+      <c r="M19" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="N19" s="34"/>
+      <c r="O19" s="34"/>
+      <c r="P19" s="34"/>
+      <c r="Q19" s="34"/>
+      <c r="R19" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="S19" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="T19" s="36"/>
+      <c r="U19" s="36"/>
+      <c r="V19" s="36"/>
+      <c r="W19" s="36"/>
+      <c r="X19" s="36"/>
+    </row>
+    <row r="20" spans="2:24" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="34"/>
+      <c r="N20" s="34"/>
+      <c r="O20" s="34"/>
+      <c r="P20" s="34"/>
+      <c r="Q20" s="34"/>
+      <c r="R20" s="34"/>
+      <c r="S20" s="34"/>
+      <c r="T20" s="36"/>
+      <c r="U20" s="36"/>
+      <c r="V20" s="36"/>
+      <c r="W20" s="36"/>
+      <c r="X20" s="36"/>
+    </row>
+    <row r="21" spans="2:24" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="34"/>
+      <c r="N21" s="34"/>
+      <c r="O21" s="34"/>
+      <c r="P21" s="34"/>
+      <c r="Q21" s="34"/>
+      <c r="R21" s="34"/>
+      <c r="S21" s="34"/>
+      <c r="T21" s="36"/>
+      <c r="U21" s="36"/>
+      <c r="V21" s="36"/>
+      <c r="W21" s="36"/>
+      <c r="X21" s="36"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>